<commit_message>
Change Excel and Excersice
</commit_message>
<xml_diff>
--- a/Control Económico.xlsx
+++ b/Control Económico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genry Luis\Documents\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C356F7B1-F3B0-4E32-A532-77E1D28937B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99567689-5693-453D-9D48-01BC334F0C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>CONTROL DE SUELDOS</t>
   </si>
@@ -140,6 +140,27 @@
   <si>
     <t>Cemaco (galletas y coca)</t>
   </si>
+  <si>
+    <t>Piezas Pollo</t>
+  </si>
+  <si>
+    <t>Amburguesa Macdonals</t>
+  </si>
+  <si>
+    <t>Super octubre</t>
+  </si>
+  <si>
+    <t>Gastos personales</t>
+  </si>
+  <si>
+    <t>Sueldo quincenal 1</t>
+  </si>
+  <si>
+    <t>Playera Naruto Uzumaky</t>
+  </si>
+  <si>
+    <t>Para tortillas pendientes</t>
+  </si>
 </sst>
 </file>
 
@@ -238,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -274,6 +295,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2968,10 +2990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4178EBF9-3FF0-4226-BA71-7DF463DFD99B}">
-  <dimension ref="B2:X93"/>
+  <dimension ref="B2:X96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2984,6 +3006,7 @@
     <col min="6" max="6" width="34.81640625" customWidth="1"/>
     <col min="7" max="7" width="11.08984375" customWidth="1"/>
     <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.35">
@@ -3057,7 +3080,7 @@
         <v>2022.22</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D4" s="14">
         <f>SUM(B4:B5)</f>
@@ -3126,7 +3149,9 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6"/>
+      <c r="B6" s="13">
+        <v>2110</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="8"/>
       <c r="E6" s="7">
@@ -3285,10 +3310,14 @@
       <c r="C11" s="6"/>
       <c r="D11" s="8"/>
       <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="9">
+        <v>44842</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3307,15 +3336,19 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="7">
+        <v>50</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="9">
+        <v>44843</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -3334,15 +3367,19 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="10"/>
+        <v>48</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="9">
+        <v>44843</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -3361,15 +3398,19 @@
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="15">
-        <v>0</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="E14" s="7">
+        <v>50</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="9">
+        <v>44844</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -3391,12 +3432,16 @@
     <row r="15" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8">
+        <v>40</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="9">
+        <v>44846</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -3418,12 +3463,16 @@
     <row r="16" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
+        <v>60</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="9">
+        <v>44846</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -3445,11 +3494,19 @@
     <row r="17" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" s="16"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6">
+        <v>30</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="9">
+        <v>44847</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="1"/>
@@ -3468,12 +3525,16 @@
     <row r="18" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="6">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="9">
+        <v>44848</v>
+      </c>
       <c r="H18" s="6"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -3496,19 +3557,17 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="14">
-        <f>SUM(E4:E18)</f>
-        <v>640</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="13">
-        <f>D4-E19</f>
-        <v>1532.2200000000003</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E19" s="6">
+        <v>100</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="9">
+        <v>44849</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -3526,20 +3585,18 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="13">
-        <f>SUM(E19:H19)</f>
-        <v>2172.2200000000003</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6">
+        <v>50</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="9">
+        <v>44849</v>
+      </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="1"/>
@@ -3556,17 +3613,17 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -3581,17 +3638,25 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="14">
+        <f>SUM(E4:E21)</f>
+        <v>1248</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="13">
+        <f>D4-E22</f>
+        <v>924.22000000000025</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -3606,19 +3671,22 @@
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1">
-        <v>1533.03</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="13">
+        <f>SUM(E22:H22)</f>
+        <v>2172.2200000000003</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -3689,7 +3757,9 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="1">
+        <v>1533.03</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -5382,7 +5452,83 @@
       <c r="W93" s="1"/>
       <c r="X93" s="1"/>
     </row>
+    <row r="94" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+    </row>
+    <row r="95" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+    </row>
+    <row r="96" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change Gestions - SQL
</commit_message>
<xml_diff>
--- a/Control Económico.xlsx
+++ b/Control Económico.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genry Luis\Documents\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A1DC6C-316D-45EB-B60F-A12D4EE5F392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EF7D39-539A-4B0C-BF1E-FAEC06ED3729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Septiembre" sheetId="1" r:id="rId1"/>
     <sheet name="Octubre" sheetId="3" r:id="rId2"/>
+    <sheet name="Noviembre" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>CONTROL DE SUELDOS</t>
   </si>
@@ -189,10 +190,58 @@
     <t>Gasolina viaje a casa</t>
   </si>
   <si>
+    <t>SALDO INICIAL</t>
+  </si>
+  <si>
+    <t>Don Calzone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gasolina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Desayuno</t>
+  </si>
+  <si>
+    <t>Crea nivea</t>
+  </si>
+  <si>
+    <t>Uso de tarjeta</t>
+  </si>
+  <si>
+    <t>No se sabe</t>
+  </si>
+  <si>
+    <t>2da-15na octubre</t>
+  </si>
+  <si>
+    <t>1ra-15na noviembre</t>
+  </si>
+  <si>
     <t>pendiente</t>
   </si>
   <si>
-    <t>SALDO INICIAL</t>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>Pago moto Suzuki</t>
+  </si>
+  <si>
+    <t>Reparación Moto Suzuki</t>
+  </si>
+  <si>
+    <t>Crema Nivea</t>
+  </si>
+  <si>
+    <t>Pedido en Temu</t>
+  </si>
+  <si>
+    <t>Burger King desayuno</t>
+  </si>
+  <si>
+    <t>Pendiente en que</t>
   </si>
 </sst>
 </file>
@@ -247,7 +296,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +309,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -295,11 +350,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -337,6 +418,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3031,10 +3120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4178EBF9-3FF0-4226-BA71-7DF463DFD99B}">
-  <dimension ref="B2:X105"/>
+  <dimension ref="B2:X114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3047,7 +3136,7 @@
     <col min="6" max="6" width="34.81640625" customWidth="1"/>
     <col min="7" max="7" width="11.08984375" customWidth="1"/>
     <col min="8" max="8" width="13.26953125" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.35">
@@ -3085,7 +3174,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>2</v>
@@ -3908,13 +3997,13 @@
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6">
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>50</v>
+      <c r="G29" s="9">
+        <v>44863</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="5"/>
@@ -3938,9 +4027,15 @@
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="9"/>
+      <c r="E30" s="6">
+        <v>20</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="9">
+        <v>44863</v>
+      </c>
       <c r="H30" s="6"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -3963,19 +4058,17 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="14">
-        <f>SUM(E4:E30)</f>
-        <v>2363</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="13">
-        <f>D4-E31</f>
-        <v>1919.2200000000003</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E31" s="6">
+        <v>20</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="9">
+        <v>44864</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -3993,22 +4086,3052 @@
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6">
         <v>10</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="13">
-        <f>SUM(E31:H31)</f>
-        <v>4282.22</v>
-      </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="F32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="9">
+        <v>44865</v>
+      </c>
       <c r="H32" s="6"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="19">
+        <v>50</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="9">
+        <v>44865</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="19">
+        <v>30</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" s="9">
+        <v>45964</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6">
+        <v>200</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="9">
+        <v>45964</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6">
+        <v>150</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="9">
+        <v>45964</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6">
+        <v>15</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="9">
+        <v>45964</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6">
+        <v>10</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="14">
+        <f>SUM(E4:E39)</f>
+        <v>3052</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="22">
+        <f>D4-E40</f>
+        <v>1230.2200000000003</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="23"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="13">
+        <f>SUM(E40:H40)</f>
+        <v>4282.22</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1">
+        <v>1533.03</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+    </row>
+    <row r="45" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+    </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+    </row>
+    <row r="47" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+    </row>
+    <row r="52" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+    </row>
+    <row r="55" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+    </row>
+    <row r="56" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+    </row>
+    <row r="57" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+    </row>
+    <row r="58" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+    </row>
+    <row r="59" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+    </row>
+    <row r="60" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+    </row>
+    <row r="61" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+    </row>
+    <row r="62" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+    </row>
+    <row r="63" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+    </row>
+    <row r="64" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+    </row>
+    <row r="65" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+    </row>
+    <row r="66" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+    </row>
+    <row r="67" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+    </row>
+    <row r="68" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+    </row>
+    <row r="69" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+    </row>
+    <row r="70" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+    </row>
+    <row r="71" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+    </row>
+    <row r="72" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+    </row>
+    <row r="73" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+    </row>
+    <row r="74" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+    </row>
+    <row r="75" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+    </row>
+    <row r="76" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+    </row>
+    <row r="77" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+    </row>
+    <row r="78" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+    </row>
+    <row r="79" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+    </row>
+    <row r="80" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+    </row>
+    <row r="81" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+    </row>
+    <row r="82" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="W82" s="1"/>
+      <c r="X82" s="1"/>
+    </row>
+    <row r="83" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+    </row>
+    <row r="84" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+    </row>
+    <row r="85" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+    </row>
+    <row r="86" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+    </row>
+    <row r="87" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="1"/>
+      <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+    </row>
+    <row r="88" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+    </row>
+    <row r="89" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="1"/>
+      <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+      <c r="W89" s="1"/>
+      <c r="X89" s="1"/>
+    </row>
+    <row r="90" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="1"/>
+      <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+    </row>
+    <row r="91" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+    </row>
+    <row r="92" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="W92" s="1"/>
+      <c r="X92" s="1"/>
+    </row>
+    <row r="93" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="1"/>
+      <c r="S93" s="1"/>
+      <c r="T93" s="1"/>
+      <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
+      <c r="W93" s="1"/>
+      <c r="X93" s="1"/>
+    </row>
+    <row r="94" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+    </row>
+    <row r="95" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+    </row>
+    <row r="96" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+    </row>
+    <row r="97" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="1"/>
+      <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+    </row>
+    <row r="98" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1"/>
+      <c r="S98" s="1"/>
+      <c r="T98" s="1"/>
+      <c r="U98" s="1"/>
+      <c r="V98" s="1"/>
+      <c r="W98" s="1"/>
+      <c r="X98" s="1"/>
+    </row>
+    <row r="99" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="1"/>
+      <c r="S99" s="1"/>
+      <c r="T99" s="1"/>
+      <c r="U99" s="1"/>
+      <c r="V99" s="1"/>
+      <c r="W99" s="1"/>
+      <c r="X99" s="1"/>
+    </row>
+    <row r="100" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
+      <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+    </row>
+    <row r="101" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+    </row>
+    <row r="102" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="1"/>
+      <c r="U102" s="1"/>
+      <c r="V102" s="1"/>
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+    </row>
+    <row r="103" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+      <c r="S103" s="1"/>
+      <c r="T103" s="1"/>
+      <c r="U103" s="1"/>
+      <c r="V103" s="1"/>
+      <c r="W103" s="1"/>
+      <c r="X103" s="1"/>
+    </row>
+    <row r="104" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="1"/>
+      <c r="T104" s="1"/>
+      <c r="U104" s="1"/>
+      <c r="V104" s="1"/>
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
+    </row>
+    <row r="105" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+    </row>
+    <row r="106" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="1"/>
+      <c r="S106" s="1"/>
+      <c r="T106" s="1"/>
+      <c r="U106" s="1"/>
+      <c r="V106" s="1"/>
+      <c r="W106" s="1"/>
+      <c r="X106" s="1"/>
+    </row>
+    <row r="107" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
+      <c r="P107" s="1"/>
+      <c r="Q107" s="1"/>
+      <c r="R107" s="1"/>
+      <c r="S107" s="1"/>
+      <c r="T107" s="1"/>
+      <c r="U107" s="1"/>
+      <c r="V107" s="1"/>
+      <c r="W107" s="1"/>
+      <c r="X107" s="1"/>
+    </row>
+    <row r="108" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+      <c r="S108" s="1"/>
+      <c r="T108" s="1"/>
+      <c r="U108" s="1"/>
+      <c r="V108" s="1"/>
+      <c r="W108" s="1"/>
+      <c r="X108" s="1"/>
+    </row>
+    <row r="109" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+      <c r="S109" s="1"/>
+      <c r="T109" s="1"/>
+      <c r="U109" s="1"/>
+      <c r="V109" s="1"/>
+      <c r="W109" s="1"/>
+      <c r="X109" s="1"/>
+    </row>
+    <row r="110" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+      <c r="R110" s="1"/>
+      <c r="S110" s="1"/>
+      <c r="T110" s="1"/>
+      <c r="U110" s="1"/>
+      <c r="V110" s="1"/>
+      <c r="W110" s="1"/>
+      <c r="X110" s="1"/>
+    </row>
+    <row r="111" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1"/>
+      <c r="P111" s="1"/>
+      <c r="Q111" s="1"/>
+      <c r="R111" s="1"/>
+      <c r="S111" s="1"/>
+      <c r="T111" s="1"/>
+      <c r="U111" s="1"/>
+      <c r="V111" s="1"/>
+      <c r="W111" s="1"/>
+      <c r="X111" s="1"/>
+    </row>
+    <row r="112" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+      <c r="R112" s="1"/>
+      <c r="S112" s="1"/>
+      <c r="T112" s="1"/>
+      <c r="U112" s="1"/>
+      <c r="V112" s="1"/>
+      <c r="W112" s="1"/>
+      <c r="X112" s="1"/>
+    </row>
+    <row r="113" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+      <c r="R113" s="1"/>
+      <c r="S113" s="1"/>
+      <c r="T113" s="1"/>
+      <c r="U113" s="1"/>
+      <c r="V113" s="1"/>
+      <c r="W113" s="1"/>
+      <c r="X113" s="1"/>
+    </row>
+    <row r="114" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+      <c r="P114" s="1"/>
+      <c r="Q114" s="1"/>
+      <c r="R114" s="1"/>
+      <c r="S114" s="1"/>
+      <c r="T114" s="1"/>
+      <c r="U114" s="1"/>
+      <c r="V114" s="1"/>
+      <c r="W114" s="1"/>
+      <c r="X114" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1400DD-AFE1-43E8-B2CF-C766C3744FCE}">
+  <dimension ref="B2:X94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="13">
+        <v>2022.22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="14">
+        <f>SUM(B4:B7)</f>
+        <v>3254.92</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2500</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="9">
+        <v>44869</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+    </row>
+    <row r="5" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="13">
+        <v>1232.7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="9">
+        <v>44869</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+    </row>
+    <row r="6" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7">
+        <v>30</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="9">
+        <v>44870</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7">
+        <v>27</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="9">
+        <v>44870</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
+        <v>212</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="9">
+        <v>44870</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
+        <v>40</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="9">
+        <v>44871</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6">
+        <v>47</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="9">
+        <v>44873</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="19">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="19">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="14">
+        <f>SUM(E4:E19)</f>
+        <v>2881</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="22">
+        <f>D4-E20</f>
+        <v>373.92000000000007</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="23"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="13">
+        <f>SUM(E20:H20)</f>
+        <v>3254.92</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1">
+        <v>1533.03</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -4079,9 +7202,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1">
-        <v>1533.03</v>
-      </c>
+      <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -5574,281 +8695,6 @@
       <c r="W94" s="1"/>
       <c r="X94" s="1"/>
     </row>
-    <row r="95" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
-      <c r="L95" s="1"/>
-      <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
-      <c r="O95" s="1"/>
-      <c r="P95" s="1"/>
-      <c r="Q95" s="1"/>
-      <c r="R95" s="1"/>
-      <c r="S95" s="1"/>
-      <c r="T95" s="1"/>
-      <c r="U95" s="1"/>
-      <c r="V95" s="1"/>
-      <c r="W95" s="1"/>
-      <c r="X95" s="1"/>
-    </row>
-    <row r="96" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="K96" s="1"/>
-      <c r="L96" s="1"/>
-      <c r="M96" s="1"/>
-      <c r="N96" s="1"/>
-      <c r="O96" s="1"/>
-      <c r="P96" s="1"/>
-      <c r="Q96" s="1"/>
-      <c r="R96" s="1"/>
-      <c r="S96" s="1"/>
-      <c r="T96" s="1"/>
-      <c r="U96" s="1"/>
-      <c r="V96" s="1"/>
-      <c r="W96" s="1"/>
-      <c r="X96" s="1"/>
-    </row>
-    <row r="97" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-      <c r="K97" s="1"/>
-      <c r="L97" s="1"/>
-      <c r="M97" s="1"/>
-      <c r="N97" s="1"/>
-      <c r="O97" s="1"/>
-      <c r="P97" s="1"/>
-      <c r="Q97" s="1"/>
-      <c r="R97" s="1"/>
-      <c r="S97" s="1"/>
-      <c r="T97" s="1"/>
-      <c r="U97" s="1"/>
-      <c r="V97" s="1"/>
-      <c r="W97" s="1"/>
-      <c r="X97" s="1"/>
-    </row>
-    <row r="98" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
-      <c r="K98" s="1"/>
-      <c r="L98" s="1"/>
-      <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
-      <c r="O98" s="1"/>
-      <c r="P98" s="1"/>
-      <c r="Q98" s="1"/>
-      <c r="R98" s="1"/>
-      <c r="S98" s="1"/>
-      <c r="T98" s="1"/>
-      <c r="U98" s="1"/>
-      <c r="V98" s="1"/>
-      <c r="W98" s="1"/>
-      <c r="X98" s="1"/>
-    </row>
-    <row r="99" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-      <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
-      <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
-      <c r="O99" s="1"/>
-      <c r="P99" s="1"/>
-      <c r="Q99" s="1"/>
-      <c r="R99" s="1"/>
-      <c r="S99" s="1"/>
-      <c r="T99" s="1"/>
-      <c r="U99" s="1"/>
-      <c r="V99" s="1"/>
-      <c r="W99" s="1"/>
-      <c r="X99" s="1"/>
-    </row>
-    <row r="100" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-      <c r="S100" s="1"/>
-      <c r="T100" s="1"/>
-      <c r="U100" s="1"/>
-      <c r="V100" s="1"/>
-      <c r="W100" s="1"/>
-      <c r="X100" s="1"/>
-    </row>
-    <row r="101" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
-      <c r="P101" s="1"/>
-      <c r="Q101" s="1"/>
-      <c r="R101" s="1"/>
-      <c r="S101" s="1"/>
-      <c r="T101" s="1"/>
-      <c r="U101" s="1"/>
-      <c r="V101" s="1"/>
-      <c r="W101" s="1"/>
-      <c r="X101" s="1"/>
-    </row>
-    <row r="102" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
-      <c r="P102" s="1"/>
-      <c r="Q102" s="1"/>
-      <c r="R102" s="1"/>
-      <c r="S102" s="1"/>
-      <c r="T102" s="1"/>
-      <c r="U102" s="1"/>
-      <c r="V102" s="1"/>
-      <c r="W102" s="1"/>
-      <c r="X102" s="1"/>
-    </row>
-    <row r="103" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-      <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-      <c r="O103" s="1"/>
-      <c r="P103" s="1"/>
-      <c r="Q103" s="1"/>
-      <c r="R103" s="1"/>
-      <c r="S103" s="1"/>
-      <c r="T103" s="1"/>
-      <c r="U103" s="1"/>
-      <c r="V103" s="1"/>
-      <c r="W103" s="1"/>
-      <c r="X103" s="1"/>
-    </row>
-    <row r="104" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
-      <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
-      <c r="O104" s="1"/>
-      <c r="P104" s="1"/>
-      <c r="Q104" s="1"/>
-      <c r="R104" s="1"/>
-      <c r="S104" s="1"/>
-      <c r="T104" s="1"/>
-      <c r="U104" s="1"/>
-      <c r="V104" s="1"/>
-      <c r="W104" s="1"/>
-      <c r="X104" s="1"/>
-    </row>
-    <row r="105" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-      <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
-      <c r="M105" s="1"/>
-      <c r="N105" s="1"/>
-      <c r="O105" s="1"/>
-      <c r="P105" s="1"/>
-      <c r="Q105" s="1"/>
-      <c r="R105" s="1"/>
-      <c r="S105" s="1"/>
-      <c r="T105" s="1"/>
-      <c r="U105" s="1"/>
-      <c r="V105" s="1"/>
-      <c r="W105" s="1"/>
-      <c r="X105" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
change in new laptop
</commit_message>
<xml_diff>
--- a/Control Económico.xlsx
+++ b/Control Económico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genry Luis\Documents\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262E0A76-573C-4183-B403-2CEAF5387356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B6259F-F638-4F85-9680-48D98A7121EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="191">
   <si>
     <t>CONTROL DE SUELDOS</t>
   </si>
@@ -569,6 +569,54 @@
   <si>
     <t>(Verduras, Cancha, Pastel)</t>
   </si>
+  <si>
+    <t>Tornillo - Física</t>
+  </si>
+  <si>
+    <t>Personaje Naruto</t>
+  </si>
+  <si>
+    <t>Gasolina para la semana</t>
+  </si>
+  <si>
+    <t>Retiro - Las brisas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibli y Guias </t>
+  </si>
+  <si>
+    <t>Retiro Gastos personales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tes </t>
+  </si>
+  <si>
+    <t>Uber de U a la casa</t>
+  </si>
+  <si>
+    <t>Instalación de Sopt Moto</t>
+  </si>
+  <si>
+    <t>Cancha sintética</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inversiones </t>
+  </si>
+  <si>
+    <t>Gasolina para fin de semana</t>
+  </si>
+  <si>
+    <t>Reparación de moto - Richard</t>
+  </si>
+  <si>
+    <t>Personajes One Piece</t>
+  </si>
+  <si>
+    <t>Piezas de Granjero</t>
+  </si>
+  <si>
+    <t>Mensualidad Universidad Febrero</t>
+  </si>
 </sst>
 </file>
 
@@ -719,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -785,6 +833,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -9602,15 +9653,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -10622,11 +10673,11 @@
         <f>D4-E31</f>
         <v>2090.8999999999996</v>
       </c>
-      <c r="I31" s="34" t="s">
+      <c r="I31" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
       <c r="L31" s="5"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -12532,16 +12583,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -14174,11 +14225,11 @@
         <f>E4-F48</f>
         <v>25.569999999999709</v>
       </c>
-      <c r="J48" s="34" t="s">
+      <c r="J48" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
       <c r="M48" s="5"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -16066,10 +16117,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F886ECA7-820D-4BE1-9837-EFDF67FD3DBB}">
-  <dimension ref="B2:Y94"/>
+  <dimension ref="B2:Y109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16088,16 +16139,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -16168,8 +16219,8 @@
         <v>46017</v>
       </c>
       <c r="E4" s="14">
-        <f>SUM(B4:B7)</f>
-        <v>1779.62</v>
+        <f>SUM(B4:B10)</f>
+        <v>3915.66</v>
       </c>
       <c r="F4" s="8">
         <v>30</v>
@@ -16182,7 +16233,7 @@
       </c>
       <c r="I4" s="6">
         <f>(E4-F4)</f>
-        <v>1749.62</v>
+        <v>3885.66</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -16223,7 +16274,7 @@
       </c>
       <c r="I5" s="6">
         <f>I4-F5</f>
-        <v>1724.62</v>
+        <v>3860.66</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -16264,7 +16315,7 @@
       </c>
       <c r="I6" s="6">
         <f>I5-F6</f>
-        <v>1624.62</v>
+        <v>3760.66</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -16284,13 +16335,15 @@
       <c r="Y6" s="1"/>
     </row>
     <row r="7" spans="2:25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
-        <v>114</v>
+      <c r="B7" s="33">
+        <v>2136.04</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="9">
+        <v>46066</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="F7" s="32">
         <v>600</v>
@@ -16303,7 +16356,7 @@
       </c>
       <c r="I7" s="6">
         <f>I6-F7</f>
-        <v>1024.6199999999999</v>
+        <v>3160.66</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -16323,7 +16376,7 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B8" s="6"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -16336,9 +16389,9 @@
       <c r="H8" s="9">
         <v>46053</v>
       </c>
-      <c r="I8" s="6" t="e">
-        <f>#REF!-F8</f>
-        <v>#REF!</v>
+      <c r="I8" s="6">
+        <f t="shared" ref="I8:I31" si="0">I7-F8</f>
+        <v>3135.66</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -16371,9 +16424,9 @@
       <c r="H9" s="9">
         <v>46054</v>
       </c>
-      <c r="I9" s="6" t="e">
-        <f t="shared" ref="I9:I18" si="0">I8-F9</f>
-        <v>#REF!</v>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
+        <v>3068.66</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -16406,9 +16459,9 @@
       <c r="H10" s="9">
         <v>46055</v>
       </c>
-      <c r="I10" s="6" t="e">
+      <c r="I10" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>3028.66</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -16438,10 +16491,12 @@
       <c r="G11" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="6" t="e">
+      <c r="H11" s="9">
+        <v>46055</v>
+      </c>
+      <c r="I11" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2928.66</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -16471,10 +16526,12 @@
       <c r="G12" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="6" t="e">
+      <c r="H12" s="9">
+        <v>46057</v>
+      </c>
+      <c r="I12" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2808.66</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -16498,12 +16555,18 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="6" t="e">
+      <c r="F13" s="6">
+        <v>18</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13" s="9">
+        <v>46057</v>
+      </c>
+      <c r="I13" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2790.66</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -16527,12 +16590,18 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="6" t="e">
+      <c r="F14" s="1">
+        <v>50</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" s="9">
+        <v>46057</v>
+      </c>
+      <c r="I14" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2740.66</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -16556,12 +16625,18 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="6" t="e">
+      <c r="F15" s="6">
+        <v>50</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="H15" s="9">
+        <v>46060</v>
+      </c>
+      <c r="I15" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2690.66</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -16585,12 +16660,18 @@
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="6" t="e">
+      <c r="F16" s="6">
+        <v>50</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="9">
+        <v>46060</v>
+      </c>
+      <c r="I16" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2640.66</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -16614,12 +16695,18 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="6" t="e">
+      <c r="F17" s="6">
+        <v>40</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H17" s="9">
+        <v>46062</v>
+      </c>
+      <c r="I17" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2600.66</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -16643,12 +16730,18 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="6" t="e">
+      <c r="F18" s="6">
+        <v>206</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="9">
+        <v>46062</v>
+      </c>
+      <c r="I18" s="6">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>2394.66</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -16672,10 +16765,19 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="20"/>
+      <c r="F19" s="6">
+        <v>35</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="H19" s="9">
+        <v>46062</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="0"/>
+        <v>2359.66</v>
+      </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -16694,27 +16796,26 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B20" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="14">
-        <f>SUM(F4:F19)</f>
-        <v>1107</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="22">
-        <f>E4-F20</f>
-        <v>672.61999999999989</v>
-      </c>
-      <c r="J20" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
+      <c r="F20" s="6">
+        <v>25</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20" s="9">
+        <v>46062</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="0"/>
+        <v>2334.66</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -16730,19 +16831,23 @@
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="13">
-        <f>SUM(F20:I20)</f>
-        <v>1779.62</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="21"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6">
+        <v>30</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H21" s="9">
+        <v>46065</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="0"/>
+        <v>2304.66</v>
+      </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -16761,17 +16866,27 @@
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6">
+        <v>20</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="9">
+        <v>46065</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="0"/>
+        <v>2284.66</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -16786,17 +16901,27 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6">
+        <v>40</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H23" s="9">
+        <v>46065</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="0"/>
+        <v>2244.66</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -16811,22 +16936,27 @@
       <c r="Y23" s="1"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1">
-        <v>1533.03</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6">
+        <v>41</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="9">
+        <v>46065</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="0"/>
+        <v>2203.66</v>
+      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -16841,17 +16971,27 @@
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="9">
+        <v>46066</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="0"/>
+        <v>2193.16</v>
+      </c>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -16866,17 +17006,27 @@
       <c r="Y25" s="1"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6">
+        <v>20</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="H26" s="9">
+        <v>46067</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="0"/>
+        <v>2173.16</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -16891,17 +17041,27 @@
       <c r="Y26" s="1"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6">
+        <v>100</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H27" s="9">
+        <v>46067</v>
+      </c>
+      <c r="I27" s="6">
+        <f t="shared" si="0"/>
+        <v>2073.16</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -16916,17 +17076,27 @@
       <c r="Y27" s="1"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6">
+        <v>117</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="H28" s="9">
+        <v>46068</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="0"/>
+        <v>1956.1599999999999</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -16941,17 +17111,27 @@
       <c r="Y28" s="1"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6">
+        <v>20</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H29" s="9">
+        <v>46068</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="0"/>
+        <v>1936.1599999999999</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -16966,17 +17146,27 @@
       <c r="Y29" s="1"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6">
+        <v>200</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="9">
+        <v>46068</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="0"/>
+        <v>1736.1599999999999</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -16991,17 +17181,27 @@
       <c r="Y30" s="1"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6">
+        <v>1153</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="H31" s="9">
+        <v>46069</v>
+      </c>
+      <c r="I31" s="6">
+        <f t="shared" si="0"/>
+        <v>583.15999999999985</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -17016,17 +17216,18 @@
       <c r="Y31" s="1"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -17041,17 +17242,18 @@
       <c r="Y32" s="1"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -17066,17 +17268,18 @@
       <c r="Y33" s="1"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -17091,17 +17294,28 @@
       <c r="Y34" s="1"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
+      <c r="B35" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="14">
+        <f>SUM(F4:F34)</f>
+        <v>3332.5</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="22">
+        <f>E4-F35</f>
+        <v>583.15999999999985</v>
+      </c>
+      <c r="J35" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="5"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -17116,17 +17330,23 @@
       <c r="Y35" s="1"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
+      <c r="B36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="13">
+        <f>SUM(F35:I35)</f>
+        <v>3915.66</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -17195,9 +17415,14 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="I39" s="1">
+        <v>1533.03</v>
+      </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -17245,6 +17470,9 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -18590,10 +18818,385 @@
       <c r="X94" s="1"/>
       <c r="Y94" s="1"/>
     </row>
+    <row r="95" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
+    </row>
+    <row r="96" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
+    </row>
+    <row r="97" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="1"/>
+      <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+      <c r="Y97" s="1"/>
+    </row>
+    <row r="98" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1"/>
+      <c r="S98" s="1"/>
+      <c r="T98" s="1"/>
+      <c r="U98" s="1"/>
+      <c r="V98" s="1"/>
+      <c r="W98" s="1"/>
+      <c r="X98" s="1"/>
+      <c r="Y98" s="1"/>
+    </row>
+    <row r="99" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="1"/>
+      <c r="S99" s="1"/>
+      <c r="T99" s="1"/>
+      <c r="U99" s="1"/>
+      <c r="V99" s="1"/>
+      <c r="W99" s="1"/>
+      <c r="X99" s="1"/>
+      <c r="Y99" s="1"/>
+    </row>
+    <row r="100" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
+      <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+      <c r="Y100" s="1"/>
+    </row>
+    <row r="101" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+    </row>
+    <row r="102" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="1"/>
+      <c r="U102" s="1"/>
+      <c r="V102" s="1"/>
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+      <c r="Y102" s="1"/>
+    </row>
+    <row r="103" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+      <c r="S103" s="1"/>
+      <c r="T103" s="1"/>
+      <c r="U103" s="1"/>
+      <c r="V103" s="1"/>
+      <c r="W103" s="1"/>
+      <c r="X103" s="1"/>
+      <c r="Y103" s="1"/>
+    </row>
+    <row r="104" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="1"/>
+      <c r="T104" s="1"/>
+      <c r="U104" s="1"/>
+      <c r="V104" s="1"/>
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
+      <c r="Y104" s="1"/>
+    </row>
+    <row r="105" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+    </row>
+    <row r="106" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="1"/>
+      <c r="S106" s="1"/>
+      <c r="T106" s="1"/>
+      <c r="U106" s="1"/>
+      <c r="V106" s="1"/>
+      <c r="W106" s="1"/>
+      <c r="X106" s="1"/>
+      <c r="Y106" s="1"/>
+    </row>
+    <row r="107" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
+      <c r="P107" s="1"/>
+      <c r="Q107" s="1"/>
+      <c r="R107" s="1"/>
+      <c r="S107" s="1"/>
+      <c r="T107" s="1"/>
+      <c r="U107" s="1"/>
+      <c r="V107" s="1"/>
+      <c r="W107" s="1"/>
+      <c r="X107" s="1"/>
+      <c r="Y107" s="1"/>
+    </row>
+    <row r="108" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+      <c r="S108" s="1"/>
+      <c r="T108" s="1"/>
+      <c r="U108" s="1"/>
+      <c r="V108" s="1"/>
+      <c r="W108" s="1"/>
+      <c r="X108" s="1"/>
+      <c r="Y108" s="1"/>
+    </row>
+    <row r="109" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+      <c r="S109" s="1"/>
+      <c r="T109" s="1"/>
+      <c r="U109" s="1"/>
+      <c r="V109" s="1"/>
+      <c r="W109" s="1"/>
+      <c r="X109" s="1"/>
+      <c r="Y109" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J35:L35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -18608,7 +19211,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" customWidth="1"/>
     <col min="2" max="3" width="24.1796875" customWidth="1"/>
@@ -18617,11 +19220,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="26" t="s">
@@ -18726,7 +19329,7 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" customWidth="1"/>
     <col min="2" max="2" width="16.54296875" customWidth="1"/>
@@ -18738,15 +19341,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="26" t="s">

</xml_diff>